<commit_message>
feat: Add new ASP.NET Minimal API tests and an exporter script, and update existing tests and content files.
</commit_message>
<xml_diff>
--- a/tests/13.aspnet/01.minimal-api/01.introduction.xlsx
+++ b/tests/13.aspnet/01.minimal-api/01.introduction.xlsx
@@ -510,15 +510,11 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>45</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
@@ -559,15 +555,11 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>30</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
@@ -608,15 +600,11 @@
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>60</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
@@ -657,15 +645,11 @@
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>45</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
@@ -706,15 +690,11 @@
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>45</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
@@ -736,22 +716,16 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Top-Level Statements</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>45</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
@@ -773,22 +747,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Middleware</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>45</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
@@ -821,15 +789,11 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>30</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
@@ -870,15 +834,11 @@
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>30</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
@@ -904,10 +864,8 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="I11" t="n">
+        <v>60</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">

</xml_diff>